<commit_message>
changed pilot/Windows/lifetime.m output behavioral filename to conform to BIDS naming scheme. Started coding for lifetime pilot analysis script
</commit_message>
<xml_diff>
--- a/stmuli/genetic_180.xlsx
+++ b/stmuli/genetic_180.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F9F729-F97C-492F-86FD-196343D03D4A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68473539-A96B-4C5B-A8C4-6EA5DB62A077}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10sets0f18" sheetId="1" r:id="rId1"/>
@@ -13,18 +13,18 @@
     <sheet name="version 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'10sets0f18'!$Y$2:$Y$19</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'10sets0f18'!$C$2:$C$19</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'10sets0f18'!$N$2:$N$19</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'10sets0f18'!$AJ$2:$AJ$19</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'10sets0f18'!$BQ$2:$BQ$19</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'10sets0f18'!$CM$2:$CM$19</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'10sets0f18'!$CX$2:$CX$19</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'10sets0f18'!$AU$2:$AU$19</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'10sets0f18'!$CB$2:$CB$19</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'10sets0f18'!$BF$2:$BF$19</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'10sets0f18'!$BF$2:$BF$19</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'10sets0f18'!$CX$2:$CX$19</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'10sets0f18'!$AJ$2:$AJ$19</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'10sets0f18'!$CM$2:$CM$19</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'10sets0f18'!$AU$2:$AU$19</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'10sets0f18'!$BQ$2:$BQ$19</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'10sets0f18'!$CB$2:$CB$19</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'10sets0f18'!$C$2:$C$19</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'10sets0f18'!$N$2:$N$19</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'10sets0f18'!$Y$2:$Y$19</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="193">
   <si>
     <t>concepts</t>
   </si>
@@ -602,6 +602,18 @@
   <si>
     <t>leotards</t>
   </si>
+  <si>
+    <t>animate</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
 </sst>
 </file>
 
@@ -657,87 +669,7 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="33">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1086,7 +1018,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1119,7 +1051,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1152,7 +1084,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1185,7 +1117,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1218,7 +1150,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1251,7 +1183,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1284,7 +1216,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1317,7 +1249,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1350,7 +1282,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1383,7 +1315,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -7018,8 +6950,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7639050" y="3606165"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="7989570" y="3606165"/>
+              <a:ext cx="4827270" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7096,7 +7028,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="14660880" y="3632835"/>
+              <a:off x="15266670" y="3632835"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -7174,7 +7106,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="21880830" y="3640455"/>
+              <a:off x="22486620" y="3640455"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -7252,7 +7184,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="28742640" y="3575685"/>
+              <a:off x="29348430" y="3575685"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -7330,7 +7262,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="35871150" y="3533775"/>
+              <a:off x="36476940" y="3533775"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -7408,7 +7340,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="42839640" y="3609975"/>
+              <a:off x="43445430" y="3609975"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -7486,7 +7418,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="50010060" y="3709035"/>
+              <a:off x="50615850" y="3709035"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -7564,7 +7496,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="57130950" y="3617595"/>
+              <a:off x="57736740" y="3617595"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -7642,7 +7574,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="63916560" y="3537585"/>
+              <a:off x="64522350" y="3537585"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -7939,10 +7871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DD19"/>
+  <dimension ref="A1:DE19"/>
   <sheetViews>
-    <sheetView topLeftCell="CK1" workbookViewId="0">
-      <selection activeCell="CV1" sqref="CV1:DD1"/>
+    <sheetView tabSelected="1" topLeftCell="CK1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7951,7 +7883,7 @@
     <col min="12" max="12" width="12.3671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7979,7 +7911,9 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
         <v>0</v>
@@ -8008,7 +7942,9 @@
       <c r="T1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="1"/>
+      <c r="U1" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="V1" s="1"/>
       <c r="W1" s="1" t="s">
         <v>0</v>
@@ -8037,7 +7973,9 @@
       <c r="AE1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="1"/>
+      <c r="AF1" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1" t="s">
         <v>0</v>
@@ -8066,7 +8004,9 @@
       <c r="AP1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AQ1" s="1"/>
+      <c r="AQ1" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="AR1" s="1"/>
       <c r="AS1" s="1" t="s">
         <v>0</v>
@@ -8095,6 +8035,9 @@
       <c r="BA1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="BB1" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="BD1" t="s">
         <v>0</v>
       </c>
@@ -8122,6 +8065,9 @@
       <c r="BL1" t="s">
         <v>8</v>
       </c>
+      <c r="BM1" t="s">
+        <v>189</v>
+      </c>
       <c r="BO1" t="s">
         <v>0</v>
       </c>
@@ -8149,6 +8095,9 @@
       <c r="BW1" t="s">
         <v>8</v>
       </c>
+      <c r="BX1" t="s">
+        <v>189</v>
+      </c>
       <c r="BZ1" t="s">
         <v>0</v>
       </c>
@@ -8176,6 +8125,9 @@
       <c r="CH1" t="s">
         <v>8</v>
       </c>
+      <c r="CI1" t="s">
+        <v>189</v>
+      </c>
       <c r="CK1" t="s">
         <v>0</v>
       </c>
@@ -8203,6 +8155,9 @@
       <c r="CS1" t="s">
         <v>8</v>
       </c>
+      <c r="CT1" t="s">
+        <v>189</v>
+      </c>
       <c r="CV1" t="s">
         <v>0</v>
       </c>
@@ -8230,8 +8185,11 @@
       <c r="DD1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -8259,7 +8217,9 @@
       <c r="I2" s="1">
         <v>1</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
         <v>27</v>
@@ -8288,7 +8248,9 @@
       <c r="T2" s="1">
         <v>2</v>
       </c>
-      <c r="U2" s="1"/>
+      <c r="U2" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1" t="s">
         <v>45</v>
@@ -8317,7 +8279,9 @@
       <c r="AE2" s="1">
         <v>3</v>
       </c>
-      <c r="AF2" s="1"/>
+      <c r="AF2" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1" t="s">
         <v>63</v>
@@ -8346,7 +8310,9 @@
       <c r="AP2" s="1">
         <v>4</v>
       </c>
-      <c r="AQ2" s="1"/>
+      <c r="AQ2" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="AR2" s="1"/>
       <c r="AS2" s="1" t="s">
         <v>81</v>
@@ -8375,6 +8341,9 @@
       <c r="BA2" s="1">
         <v>5</v>
       </c>
+      <c r="BB2" t="s">
+        <v>191</v>
+      </c>
       <c r="BD2" t="s">
         <v>99</v>
       </c>
@@ -8402,6 +8371,9 @@
       <c r="BL2">
         <v>6</v>
       </c>
+      <c r="BM2" t="s">
+        <v>191</v>
+      </c>
       <c r="BO2" t="s">
         <v>117</v>
       </c>
@@ -8429,6 +8401,9 @@
       <c r="BW2">
         <v>7</v>
       </c>
+      <c r="BX2" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ2" t="s">
         <v>135</v>
       </c>
@@ -8456,6 +8431,9 @@
       <c r="CH2">
         <v>8</v>
       </c>
+      <c r="CI2" t="s">
+        <v>190</v>
+      </c>
       <c r="CK2" t="s">
         <v>153</v>
       </c>
@@ -8483,6 +8461,9 @@
       <c r="CS2">
         <v>9</v>
       </c>
+      <c r="CT2" t="s">
+        <v>190</v>
+      </c>
       <c r="CV2" t="s">
         <v>171</v>
       </c>
@@ -8510,8 +8491,11 @@
       <c r="DD2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -8539,7 +8523,9 @@
       <c r="I3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
         <v>28</v>
@@ -8568,7 +8554,9 @@
       <c r="T3" s="1">
         <v>2</v>
       </c>
-      <c r="U3" s="1"/>
+      <c r="U3" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V3" s="1"/>
       <c r="W3" s="1" t="s">
         <v>46</v>
@@ -8597,7 +8585,9 @@
       <c r="AE3" s="1">
         <v>3</v>
       </c>
-      <c r="AF3" s="1"/>
+      <c r="AF3" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1" t="s">
         <v>64</v>
@@ -8626,7 +8616,9 @@
       <c r="AP3" s="1">
         <v>4</v>
       </c>
-      <c r="AQ3" s="1"/>
+      <c r="AQ3" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR3" s="1"/>
       <c r="AS3" s="1" t="s">
         <v>82</v>
@@ -8655,6 +8647,9 @@
       <c r="BA3" s="1">
         <v>5</v>
       </c>
+      <c r="BB3" t="s">
+        <v>191</v>
+      </c>
       <c r="BD3" t="s">
         <v>100</v>
       </c>
@@ -8682,6 +8677,9 @@
       <c r="BL3">
         <v>6</v>
       </c>
+      <c r="BM3" t="s">
+        <v>191</v>
+      </c>
       <c r="BO3" t="s">
         <v>118</v>
       </c>
@@ -8709,6 +8707,9 @@
       <c r="BW3">
         <v>7</v>
       </c>
+      <c r="BX3" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ3" t="s">
         <v>136</v>
       </c>
@@ -8736,6 +8737,9 @@
       <c r="CH3">
         <v>8</v>
       </c>
+      <c r="CI3" t="s">
+        <v>190</v>
+      </c>
       <c r="CK3" t="s">
         <v>154</v>
       </c>
@@ -8763,6 +8767,9 @@
       <c r="CS3">
         <v>9</v>
       </c>
+      <c r="CT3" t="s">
+        <v>191</v>
+      </c>
       <c r="CV3" t="s">
         <v>172</v>
       </c>
@@ -8790,8 +8797,11 @@
       <c r="DD3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -8819,7 +8829,9 @@
       <c r="I4" s="1">
         <v>1</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
         <v>29</v>
@@ -8848,7 +8860,9 @@
       <c r="T4" s="1">
         <v>2</v>
       </c>
-      <c r="U4" s="1"/>
+      <c r="U4" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V4" s="1"/>
       <c r="W4" s="1" t="s">
         <v>47</v>
@@ -8877,7 +8891,9 @@
       <c r="AE4" s="1">
         <v>3</v>
       </c>
-      <c r="AF4" s="1"/>
+      <c r="AF4" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1" t="s">
         <v>65</v>
@@ -8906,7 +8922,9 @@
       <c r="AP4" s="1">
         <v>4</v>
       </c>
-      <c r="AQ4" s="1"/>
+      <c r="AQ4" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR4" s="1"/>
       <c r="AS4" s="1" t="s">
         <v>83</v>
@@ -8935,6 +8953,9 @@
       <c r="BA4" s="1">
         <v>5</v>
       </c>
+      <c r="BB4" t="s">
+        <v>191</v>
+      </c>
       <c r="BD4" t="s">
         <v>101</v>
       </c>
@@ -8962,6 +8983,9 @@
       <c r="BL4">
         <v>6</v>
       </c>
+      <c r="BM4" t="s">
+        <v>191</v>
+      </c>
       <c r="BO4" t="s">
         <v>119</v>
       </c>
@@ -8989,6 +9013,9 @@
       <c r="BW4">
         <v>7</v>
       </c>
+      <c r="BX4" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ4" t="s">
         <v>137</v>
       </c>
@@ -9016,6 +9043,9 @@
       <c r="CH4">
         <v>8</v>
       </c>
+      <c r="CI4" t="s">
+        <v>191</v>
+      </c>
       <c r="CK4" t="s">
         <v>155</v>
       </c>
@@ -9043,6 +9073,9 @@
       <c r="CS4">
         <v>9</v>
       </c>
+      <c r="CT4" t="s">
+        <v>190</v>
+      </c>
       <c r="CV4" t="s">
         <v>173</v>
       </c>
@@ -9070,8 +9103,11 @@
       <c r="DD4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -9099,7 +9135,9 @@
       <c r="I5" s="1">
         <v>1</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
         <v>30</v>
@@ -9128,7 +9166,9 @@
       <c r="T5" s="1">
         <v>2</v>
       </c>
-      <c r="U5" s="1"/>
+      <c r="U5" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1" t="s">
         <v>48</v>
@@ -9157,7 +9197,9 @@
       <c r="AE5" s="1">
         <v>3</v>
       </c>
-      <c r="AF5" s="1"/>
+      <c r="AF5" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1" t="s">
         <v>66</v>
@@ -9186,7 +9228,9 @@
       <c r="AP5" s="1">
         <v>4</v>
       </c>
-      <c r="AQ5" s="1"/>
+      <c r="AQ5" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR5" s="1"/>
       <c r="AS5" s="1" t="s">
         <v>84</v>
@@ -9215,6 +9259,9 @@
       <c r="BA5" s="1">
         <v>5</v>
       </c>
+      <c r="BB5" t="s">
+        <v>191</v>
+      </c>
       <c r="BD5" t="s">
         <v>102</v>
       </c>
@@ -9242,6 +9289,9 @@
       <c r="BL5">
         <v>6</v>
       </c>
+      <c r="BM5" t="s">
+        <v>191</v>
+      </c>
       <c r="BO5" t="s">
         <v>120</v>
       </c>
@@ -9269,6 +9319,9 @@
       <c r="BW5">
         <v>7</v>
       </c>
+      <c r="BX5" t="s">
+        <v>190</v>
+      </c>
       <c r="BZ5" t="s">
         <v>138</v>
       </c>
@@ -9296,6 +9349,9 @@
       <c r="CH5">
         <v>8</v>
       </c>
+      <c r="CI5" t="s">
+        <v>191</v>
+      </c>
       <c r="CK5" t="s">
         <v>156</v>
       </c>
@@ -9323,6 +9379,9 @@
       <c r="CS5">
         <v>9</v>
       </c>
+      <c r="CT5" t="s">
+        <v>191</v>
+      </c>
       <c r="CV5" t="s">
         <v>174</v>
       </c>
@@ -9350,8 +9409,11 @@
       <c r="DD5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -9379,7 +9441,9 @@
       <c r="I6" s="1">
         <v>1</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
         <v>31</v>
@@ -9408,7 +9472,9 @@
       <c r="T6" s="1">
         <v>2</v>
       </c>
-      <c r="U6" s="1"/>
+      <c r="U6" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1" t="s">
         <v>49</v>
@@ -9437,7 +9503,9 @@
       <c r="AE6" s="1">
         <v>3</v>
       </c>
-      <c r="AF6" s="1"/>
+      <c r="AF6" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1" t="s">
         <v>67</v>
@@ -9466,7 +9534,9 @@
       <c r="AP6" s="1">
         <v>4</v>
       </c>
-      <c r="AQ6" s="1"/>
+      <c r="AQ6" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR6" s="1"/>
       <c r="AS6" s="1" t="s">
         <v>85</v>
@@ -9495,6 +9565,9 @@
       <c r="BA6" s="1">
         <v>5</v>
       </c>
+      <c r="BB6" t="s">
+        <v>191</v>
+      </c>
       <c r="BD6" t="s">
         <v>103</v>
       </c>
@@ -9522,6 +9595,9 @@
       <c r="BL6">
         <v>6</v>
       </c>
+      <c r="BM6" t="s">
+        <v>191</v>
+      </c>
       <c r="BO6" t="s">
         <v>121</v>
       </c>
@@ -9549,6 +9625,9 @@
       <c r="BW6">
         <v>7</v>
       </c>
+      <c r="BX6" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ6" t="s">
         <v>139</v>
       </c>
@@ -9576,6 +9655,9 @@
       <c r="CH6">
         <v>8</v>
       </c>
+      <c r="CI6" t="s">
+        <v>191</v>
+      </c>
       <c r="CK6" t="s">
         <v>157</v>
       </c>
@@ -9603,6 +9685,9 @@
       <c r="CS6">
         <v>9</v>
       </c>
+      <c r="CT6" t="s">
+        <v>191</v>
+      </c>
       <c r="CV6" t="s">
         <v>175</v>
       </c>
@@ -9630,8 +9715,11 @@
       <c r="DD6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -9659,7 +9747,9 @@
       <c r="I7" s="1">
         <v>1</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1" t="s">
         <v>32</v>
@@ -9688,7 +9778,9 @@
       <c r="T7" s="1">
         <v>2</v>
       </c>
-      <c r="U7" s="1"/>
+      <c r="U7" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V7" s="1"/>
       <c r="W7" s="1" t="s">
         <v>50</v>
@@ -9717,7 +9809,9 @@
       <c r="AE7" s="1">
         <v>3</v>
       </c>
-      <c r="AF7" s="1"/>
+      <c r="AF7" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1" t="s">
         <v>68</v>
@@ -9746,7 +9840,9 @@
       <c r="AP7" s="1">
         <v>4</v>
       </c>
-      <c r="AQ7" s="1"/>
+      <c r="AQ7" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR7" s="1"/>
       <c r="AS7" s="1" t="s">
         <v>86</v>
@@ -9775,6 +9871,9 @@
       <c r="BA7" s="1">
         <v>5</v>
       </c>
+      <c r="BB7" t="s">
+        <v>191</v>
+      </c>
       <c r="BD7" t="s">
         <v>104</v>
       </c>
@@ -9802,6 +9901,9 @@
       <c r="BL7">
         <v>6</v>
       </c>
+      <c r="BM7" t="s">
+        <v>191</v>
+      </c>
       <c r="BO7" t="s">
         <v>122</v>
       </c>
@@ -9829,6 +9931,9 @@
       <c r="BW7">
         <v>7</v>
       </c>
+      <c r="BX7" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ7" t="s">
         <v>140</v>
       </c>
@@ -9856,6 +9961,9 @@
       <c r="CH7">
         <v>8</v>
       </c>
+      <c r="CI7" t="s">
+        <v>191</v>
+      </c>
       <c r="CK7" t="s">
         <v>158</v>
       </c>
@@ -9883,6 +9991,9 @@
       <c r="CS7">
         <v>9</v>
       </c>
+      <c r="CT7" t="s">
+        <v>191</v>
+      </c>
       <c r="CV7" t="s">
         <v>176</v>
       </c>
@@ -9910,8 +10021,11 @@
       <c r="DD7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -9939,7 +10053,9 @@
       <c r="I8" s="1">
         <v>1</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1" t="s">
         <v>33</v>
@@ -9968,7 +10084,9 @@
       <c r="T8" s="1">
         <v>2</v>
       </c>
-      <c r="U8" s="1"/>
+      <c r="U8" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V8" s="1"/>
       <c r="W8" s="1" t="s">
         <v>51</v>
@@ -9997,7 +10115,9 @@
       <c r="AE8" s="1">
         <v>3</v>
       </c>
-      <c r="AF8" s="1"/>
+      <c r="AF8" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="AG8" s="1"/>
       <c r="AH8" s="1" t="s">
         <v>69</v>
@@ -10026,7 +10146,9 @@
       <c r="AP8" s="1">
         <v>4</v>
       </c>
-      <c r="AQ8" s="1"/>
+      <c r="AQ8" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR8" s="1"/>
       <c r="AS8" s="1" t="s">
         <v>87</v>
@@ -10055,6 +10177,9 @@
       <c r="BA8" s="1">
         <v>5</v>
       </c>
+      <c r="BB8" t="s">
+        <v>191</v>
+      </c>
       <c r="BD8" t="s">
         <v>105</v>
       </c>
@@ -10082,6 +10207,9 @@
       <c r="BL8">
         <v>6</v>
       </c>
+      <c r="BM8" t="s">
+        <v>191</v>
+      </c>
       <c r="BO8" t="s">
         <v>123</v>
       </c>
@@ -10109,6 +10237,9 @@
       <c r="BW8">
         <v>7</v>
       </c>
+      <c r="BX8" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ8" t="s">
         <v>141</v>
       </c>
@@ -10136,6 +10267,9 @@
       <c r="CH8">
         <v>8</v>
       </c>
+      <c r="CI8" t="s">
+        <v>190</v>
+      </c>
       <c r="CK8" t="s">
         <v>159</v>
       </c>
@@ -10163,6 +10297,9 @@
       <c r="CS8">
         <v>9</v>
       </c>
+      <c r="CT8" t="s">
+        <v>191</v>
+      </c>
       <c r="CV8" t="s">
         <v>177</v>
       </c>
@@ -10190,8 +10327,11 @@
       <c r="DD8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -10219,7 +10359,9 @@
       <c r="I9" s="1">
         <v>1</v>
       </c>
-      <c r="J9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
         <v>34</v>
@@ -10248,7 +10390,9 @@
       <c r="T9" s="1">
         <v>2</v>
       </c>
-      <c r="U9" s="1"/>
+      <c r="U9" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V9" s="1"/>
       <c r="W9" s="1" t="s">
         <v>52</v>
@@ -10277,7 +10421,9 @@
       <c r="AE9" s="1">
         <v>3</v>
       </c>
-      <c r="AF9" s="1"/>
+      <c r="AF9" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG9" s="1"/>
       <c r="AH9" s="1" t="s">
         <v>70</v>
@@ -10306,7 +10452,9 @@
       <c r="AP9" s="1">
         <v>4</v>
       </c>
-      <c r="AQ9" s="1"/>
+      <c r="AQ9" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR9" s="1"/>
       <c r="AS9" s="1" t="s">
         <v>88</v>
@@ -10335,6 +10483,9 @@
       <c r="BA9" s="1">
         <v>5</v>
       </c>
+      <c r="BB9" t="s">
+        <v>191</v>
+      </c>
       <c r="BD9" t="s">
         <v>106</v>
       </c>
@@ -10362,6 +10513,9 @@
       <c r="BL9">
         <v>6</v>
       </c>
+      <c r="BM9" t="s">
+        <v>190</v>
+      </c>
       <c r="BO9" t="s">
         <v>124</v>
       </c>
@@ -10389,6 +10543,9 @@
       <c r="BW9">
         <v>7</v>
       </c>
+      <c r="BX9" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ9" t="s">
         <v>142</v>
       </c>
@@ -10416,6 +10573,9 @@
       <c r="CH9">
         <v>8</v>
       </c>
+      <c r="CI9" t="s">
+        <v>191</v>
+      </c>
       <c r="CK9" t="s">
         <v>160</v>
       </c>
@@ -10443,6 +10603,9 @@
       <c r="CS9">
         <v>9</v>
       </c>
+      <c r="CT9" t="s">
+        <v>191</v>
+      </c>
       <c r="CV9" t="s">
         <v>178</v>
       </c>
@@ -10470,8 +10633,11 @@
       <c r="DD9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -10499,7 +10665,9 @@
       <c r="I10" s="1">
         <v>1</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
         <v>35</v>
@@ -10528,7 +10696,9 @@
       <c r="T10" s="1">
         <v>2</v>
       </c>
-      <c r="U10" s="1"/>
+      <c r="U10" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V10" s="1"/>
       <c r="W10" s="1" t="s">
         <v>53</v>
@@ -10557,7 +10727,9 @@
       <c r="AE10" s="1">
         <v>3</v>
       </c>
-      <c r="AF10" s="1"/>
+      <c r="AF10" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG10" s="1"/>
       <c r="AH10" s="1" t="s">
         <v>71</v>
@@ -10586,7 +10758,9 @@
       <c r="AP10" s="1">
         <v>4</v>
       </c>
-      <c r="AQ10" s="1"/>
+      <c r="AQ10" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="AR10" s="1"/>
       <c r="AS10" s="1" t="s">
         <v>89</v>
@@ -10615,6 +10789,9 @@
       <c r="BA10" s="1">
         <v>5</v>
       </c>
+      <c r="BB10" t="s">
+        <v>191</v>
+      </c>
       <c r="BD10" t="s">
         <v>107</v>
       </c>
@@ -10642,6 +10819,9 @@
       <c r="BL10">
         <v>6</v>
       </c>
+      <c r="BM10" t="s">
+        <v>191</v>
+      </c>
       <c r="BO10" t="s">
         <v>125</v>
       </c>
@@ -10669,6 +10849,9 @@
       <c r="BW10">
         <v>7</v>
       </c>
+      <c r="BX10" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ10" t="s">
         <v>143</v>
       </c>
@@ -10696,6 +10879,9 @@
       <c r="CH10">
         <v>8</v>
       </c>
+      <c r="CI10" t="s">
+        <v>191</v>
+      </c>
       <c r="CK10" t="s">
         <v>161</v>
       </c>
@@ -10723,6 +10909,9 @@
       <c r="CS10">
         <v>9</v>
       </c>
+      <c r="CT10" t="s">
+        <v>191</v>
+      </c>
       <c r="CV10" t="s">
         <v>179</v>
       </c>
@@ -10750,8 +10939,11 @@
       <c r="DD10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -10779,7 +10971,9 @@
       <c r="I11" s="1">
         <v>1</v>
       </c>
-      <c r="J11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
         <v>36</v>
@@ -10808,7 +11002,9 @@
       <c r="T11" s="1">
         <v>2</v>
       </c>
-      <c r="U11" s="1"/>
+      <c r="U11" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V11" s="1"/>
       <c r="W11" s="1" t="s">
         <v>54</v>
@@ -10837,7 +11033,9 @@
       <c r="AE11" s="1">
         <v>3</v>
       </c>
-      <c r="AF11" s="1"/>
+      <c r="AF11" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG11" s="1"/>
       <c r="AH11" s="1" t="s">
         <v>72</v>
@@ -10866,7 +11064,9 @@
       <c r="AP11" s="1">
         <v>4</v>
       </c>
-      <c r="AQ11" s="1"/>
+      <c r="AQ11" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR11" s="1"/>
       <c r="AS11" s="1" t="s">
         <v>90</v>
@@ -10895,6 +11095,9 @@
       <c r="BA11" s="1">
         <v>5</v>
       </c>
+      <c r="BB11" t="s">
+        <v>191</v>
+      </c>
       <c r="BD11" t="s">
         <v>108</v>
       </c>
@@ -10922,6 +11125,9 @@
       <c r="BL11">
         <v>6</v>
       </c>
+      <c r="BM11" t="s">
+        <v>191</v>
+      </c>
       <c r="BO11" t="s">
         <v>126</v>
       </c>
@@ -10949,6 +11155,9 @@
       <c r="BW11">
         <v>7</v>
       </c>
+      <c r="BX11" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ11" t="s">
         <v>144</v>
       </c>
@@ -10976,6 +11185,9 @@
       <c r="CH11">
         <v>8</v>
       </c>
+      <c r="CI11" t="s">
+        <v>191</v>
+      </c>
       <c r="CK11" t="s">
         <v>162</v>
       </c>
@@ -11003,6 +11215,9 @@
       <c r="CS11">
         <v>9</v>
       </c>
+      <c r="CT11" t="s">
+        <v>191</v>
+      </c>
       <c r="CV11" t="s">
         <v>180</v>
       </c>
@@ -11030,8 +11245,11 @@
       <c r="DD11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -11059,7 +11277,9 @@
       <c r="I12" s="1">
         <v>1</v>
       </c>
-      <c r="J12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1" t="s">
         <v>37</v>
@@ -11088,7 +11308,9 @@
       <c r="T12" s="1">
         <v>2</v>
       </c>
-      <c r="U12" s="1"/>
+      <c r="U12" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V12" s="1"/>
       <c r="W12" s="1" t="s">
         <v>55</v>
@@ -11117,7 +11339,9 @@
       <c r="AE12" s="1">
         <v>3</v>
       </c>
-      <c r="AF12" s="1"/>
+      <c r="AF12" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="AG12" s="1"/>
       <c r="AH12" s="1" t="s">
         <v>73</v>
@@ -11146,7 +11370,9 @@
       <c r="AP12" s="1">
         <v>4</v>
       </c>
-      <c r="AQ12" s="1"/>
+      <c r="AQ12" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR12" s="1"/>
       <c r="AS12" s="1" t="s">
         <v>91</v>
@@ -11175,6 +11401,9 @@
       <c r="BA12" s="1">
         <v>5</v>
       </c>
+      <c r="BB12" t="s">
+        <v>191</v>
+      </c>
       <c r="BD12" t="s">
         <v>109</v>
       </c>
@@ -11202,6 +11431,9 @@
       <c r="BL12">
         <v>6</v>
       </c>
+      <c r="BM12" t="s">
+        <v>190</v>
+      </c>
       <c r="BO12" t="s">
         <v>127</v>
       </c>
@@ -11229,6 +11461,9 @@
       <c r="BW12">
         <v>7</v>
       </c>
+      <c r="BX12" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ12" t="s">
         <v>145</v>
       </c>
@@ -11256,6 +11491,9 @@
       <c r="CH12">
         <v>8</v>
       </c>
+      <c r="CI12" t="s">
+        <v>191</v>
+      </c>
       <c r="CK12" t="s">
         <v>163</v>
       </c>
@@ -11283,6 +11521,9 @@
       <c r="CS12">
         <v>9</v>
       </c>
+      <c r="CT12" t="s">
+        <v>191</v>
+      </c>
       <c r="CV12" t="s">
         <v>181</v>
       </c>
@@ -11310,8 +11551,11 @@
       <c r="DD12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
@@ -11339,7 +11583,9 @@
       <c r="I13" s="1">
         <v>1</v>
       </c>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
         <v>38</v>
@@ -11368,7 +11614,9 @@
       <c r="T13" s="1">
         <v>2</v>
       </c>
-      <c r="U13" s="1"/>
+      <c r="U13" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V13" s="1"/>
       <c r="W13" s="1" t="s">
         <v>56</v>
@@ -11397,7 +11645,9 @@
       <c r="AE13" s="1">
         <v>3</v>
       </c>
-      <c r="AF13" s="1"/>
+      <c r="AF13" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG13" s="1"/>
       <c r="AH13" s="1" t="s">
         <v>74</v>
@@ -11426,7 +11676,9 @@
       <c r="AP13" s="1">
         <v>4</v>
       </c>
-      <c r="AQ13" s="1"/>
+      <c r="AQ13" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR13" s="1"/>
       <c r="AS13" s="1" t="s">
         <v>92</v>
@@ -11455,6 +11707,9 @@
       <c r="BA13" s="1">
         <v>5</v>
       </c>
+      <c r="BB13" t="s">
+        <v>191</v>
+      </c>
       <c r="BD13" t="s">
         <v>110</v>
       </c>
@@ -11482,6 +11737,9 @@
       <c r="BL13">
         <v>6</v>
       </c>
+      <c r="BM13" t="s">
+        <v>191</v>
+      </c>
       <c r="BO13" t="s">
         <v>128</v>
       </c>
@@ -11509,6 +11767,9 @@
       <c r="BW13">
         <v>7</v>
       </c>
+      <c r="BX13" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ13" t="s">
         <v>146</v>
       </c>
@@ -11536,6 +11797,9 @@
       <c r="CH13">
         <v>8</v>
       </c>
+      <c r="CI13" t="s">
+        <v>190</v>
+      </c>
       <c r="CK13" t="s">
         <v>164</v>
       </c>
@@ -11563,6 +11827,9 @@
       <c r="CS13">
         <v>9</v>
       </c>
+      <c r="CT13" t="s">
+        <v>191</v>
+      </c>
       <c r="CV13" t="s">
         <v>182</v>
       </c>
@@ -11590,8 +11857,11 @@
       <c r="DD13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -11619,7 +11889,9 @@
       <c r="I14" s="1">
         <v>1</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
         <v>39</v>
@@ -11648,7 +11920,9 @@
       <c r="T14" s="1">
         <v>2</v>
       </c>
-      <c r="U14" s="1"/>
+      <c r="U14" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V14" s="1"/>
       <c r="W14" s="1" t="s">
         <v>57</v>
@@ -11677,7 +11951,9 @@
       <c r="AE14" s="1">
         <v>3</v>
       </c>
-      <c r="AF14" s="1"/>
+      <c r="AF14" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG14" s="1"/>
       <c r="AH14" s="1" t="s">
         <v>75</v>
@@ -11706,7 +11982,9 @@
       <c r="AP14" s="1">
         <v>4</v>
       </c>
-      <c r="AQ14" s="1"/>
+      <c r="AQ14" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR14" s="1"/>
       <c r="AS14" s="1" t="s">
         <v>93</v>
@@ -11735,6 +12013,9 @@
       <c r="BA14" s="1">
         <v>5</v>
       </c>
+      <c r="BB14" t="s">
+        <v>190</v>
+      </c>
       <c r="BD14" t="s">
         <v>111</v>
       </c>
@@ -11762,6 +12043,9 @@
       <c r="BL14">
         <v>6</v>
       </c>
+      <c r="BM14" t="s">
+        <v>191</v>
+      </c>
       <c r="BO14" t="s">
         <v>129</v>
       </c>
@@ -11789,6 +12073,9 @@
       <c r="BW14">
         <v>7</v>
       </c>
+      <c r="BX14" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ14" t="s">
         <v>147</v>
       </c>
@@ -11816,6 +12103,9 @@
       <c r="CH14">
         <v>8</v>
       </c>
+      <c r="CI14" t="s">
+        <v>191</v>
+      </c>
       <c r="CK14" t="s">
         <v>165</v>
       </c>
@@ -11843,6 +12133,9 @@
       <c r="CS14">
         <v>9</v>
       </c>
+      <c r="CT14" t="s">
+        <v>191</v>
+      </c>
       <c r="CV14" t="s">
         <v>183</v>
       </c>
@@ -11870,8 +12163,11 @@
       <c r="DD14">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -11899,7 +12195,9 @@
       <c r="I15" s="1">
         <v>1</v>
       </c>
-      <c r="J15" s="1"/>
+      <c r="J15" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
         <v>40</v>
@@ -11928,7 +12226,9 @@
       <c r="T15" s="1">
         <v>2</v>
       </c>
-      <c r="U15" s="1"/>
+      <c r="U15" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V15" s="1"/>
       <c r="W15" s="1" t="s">
         <v>58</v>
@@ -11957,7 +12257,9 @@
       <c r="AE15" s="1">
         <v>3</v>
       </c>
-      <c r="AF15" s="1"/>
+      <c r="AF15" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG15" s="1"/>
       <c r="AH15" s="1" t="s">
         <v>76</v>
@@ -11986,7 +12288,9 @@
       <c r="AP15" s="1">
         <v>4</v>
       </c>
-      <c r="AQ15" s="1"/>
+      <c r="AQ15" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR15" s="1"/>
       <c r="AS15" s="1" t="s">
         <v>94</v>
@@ -12015,6 +12319,9 @@
       <c r="BA15" s="1">
         <v>5</v>
       </c>
+      <c r="BB15" t="s">
+        <v>191</v>
+      </c>
       <c r="BD15" t="s">
         <v>112</v>
       </c>
@@ -12042,6 +12349,9 @@
       <c r="BL15">
         <v>6</v>
       </c>
+      <c r="BM15" t="s">
+        <v>190</v>
+      </c>
       <c r="BO15" t="s">
         <v>130</v>
       </c>
@@ -12069,6 +12379,9 @@
       <c r="BW15">
         <v>7</v>
       </c>
+      <c r="BX15" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ15" t="s">
         <v>148</v>
       </c>
@@ -12096,6 +12409,9 @@
       <c r="CH15">
         <v>8</v>
       </c>
+      <c r="CI15" t="s">
+        <v>191</v>
+      </c>
       <c r="CK15" t="s">
         <v>166</v>
       </c>
@@ -12123,6 +12439,9 @@
       <c r="CS15">
         <v>9</v>
       </c>
+      <c r="CT15" t="s">
+        <v>191</v>
+      </c>
       <c r="CV15" t="s">
         <v>184</v>
       </c>
@@ -12150,8 +12469,11 @@
       <c r="DD15">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -12179,7 +12501,9 @@
       <c r="I16" s="1">
         <v>1</v>
       </c>
-      <c r="J16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
         <v>41</v>
@@ -12208,7 +12532,9 @@
       <c r="T16" s="1">
         <v>2</v>
       </c>
-      <c r="U16" s="1"/>
+      <c r="U16" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V16" s="1"/>
       <c r="W16" s="1" t="s">
         <v>59</v>
@@ -12237,7 +12563,9 @@
       <c r="AE16" s="1">
         <v>3</v>
       </c>
-      <c r="AF16" s="1"/>
+      <c r="AF16" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="AG16" s="1"/>
       <c r="AH16" s="1" t="s">
         <v>77</v>
@@ -12266,7 +12594,9 @@
       <c r="AP16" s="1">
         <v>4</v>
       </c>
-      <c r="AQ16" s="1"/>
+      <c r="AQ16" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR16" s="1"/>
       <c r="AS16" s="1" t="s">
         <v>95</v>
@@ -12295,6 +12625,9 @@
       <c r="BA16" s="1">
         <v>5</v>
       </c>
+      <c r="BB16" t="s">
+        <v>191</v>
+      </c>
       <c r="BD16" t="s">
         <v>113</v>
       </c>
@@ -12322,6 +12655,9 @@
       <c r="BL16">
         <v>6</v>
       </c>
+      <c r="BM16" t="s">
+        <v>191</v>
+      </c>
       <c r="BO16" t="s">
         <v>131</v>
       </c>
@@ -12349,6 +12685,9 @@
       <c r="BW16">
         <v>7</v>
       </c>
+      <c r="BX16" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ16" t="s">
         <v>149</v>
       </c>
@@ -12376,6 +12715,9 @@
       <c r="CH16">
         <v>8</v>
       </c>
+      <c r="CI16" t="s">
+        <v>190</v>
+      </c>
       <c r="CK16" t="s">
         <v>167</v>
       </c>
@@ -12403,6 +12745,9 @@
       <c r="CS16">
         <v>9</v>
       </c>
+      <c r="CT16" t="s">
+        <v>191</v>
+      </c>
       <c r="CV16" t="s">
         <v>185</v>
       </c>
@@ -12430,8 +12775,11 @@
       <c r="DD16">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -12459,7 +12807,9 @@
       <c r="I17" s="1">
         <v>1</v>
       </c>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1" t="s">
         <v>42</v>
@@ -12488,7 +12838,9 @@
       <c r="T17" s="1">
         <v>2</v>
       </c>
-      <c r="U17" s="1"/>
+      <c r="U17" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V17" s="1"/>
       <c r="W17" s="1" t="s">
         <v>60</v>
@@ -12517,7 +12869,9 @@
       <c r="AE17" s="1">
         <v>3</v>
       </c>
-      <c r="AF17" s="1"/>
+      <c r="AF17" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG17" s="1"/>
       <c r="AH17" s="1" t="s">
         <v>78</v>
@@ -12546,7 +12900,9 @@
       <c r="AP17" s="1">
         <v>4</v>
       </c>
-      <c r="AQ17" s="1"/>
+      <c r="AQ17" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR17" s="1"/>
       <c r="AS17" s="1" t="s">
         <v>96</v>
@@ -12575,6 +12931,9 @@
       <c r="BA17" s="1">
         <v>5</v>
       </c>
+      <c r="BB17" t="s">
+        <v>191</v>
+      </c>
       <c r="BD17" t="s">
         <v>114</v>
       </c>
@@ -12602,6 +12961,9 @@
       <c r="BL17">
         <v>6</v>
       </c>
+      <c r="BM17" t="s">
+        <v>191</v>
+      </c>
       <c r="BO17" t="s">
         <v>132</v>
       </c>
@@ -12629,6 +12991,9 @@
       <c r="BW17">
         <v>7</v>
       </c>
+      <c r="BX17" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ17" t="s">
         <v>150</v>
       </c>
@@ -12656,6 +13021,9 @@
       <c r="CH17">
         <v>8</v>
       </c>
+      <c r="CI17" t="s">
+        <v>190</v>
+      </c>
       <c r="CK17" t="s">
         <v>168</v>
       </c>
@@ -12683,6 +13051,9 @@
       <c r="CS17">
         <v>9</v>
       </c>
+      <c r="CT17" t="s">
+        <v>190</v>
+      </c>
       <c r="CV17" t="s">
         <v>186</v>
       </c>
@@ -12710,8 +13081,11 @@
       <c r="DD17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -12739,7 +13113,9 @@
       <c r="I18" s="1">
         <v>1</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1" t="s">
         <v>43</v>
@@ -12768,7 +13144,9 @@
       <c r="T18" s="1">
         <v>2</v>
       </c>
-      <c r="U18" s="1"/>
+      <c r="U18" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V18" s="1"/>
       <c r="W18" s="1" t="s">
         <v>61</v>
@@ -12797,7 +13175,9 @@
       <c r="AE18" s="1">
         <v>3</v>
       </c>
-      <c r="AF18" s="1"/>
+      <c r="AF18" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AG18" s="1"/>
       <c r="AH18" s="1" t="s">
         <v>79</v>
@@ -12826,7 +13206,9 @@
       <c r="AP18" s="1">
         <v>4</v>
       </c>
-      <c r="AQ18" s="1"/>
+      <c r="AQ18" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR18" s="1"/>
       <c r="AS18" s="1" t="s">
         <v>97</v>
@@ -12855,6 +13237,9 @@
       <c r="BA18" s="1">
         <v>5</v>
       </c>
+      <c r="BB18" t="s">
+        <v>191</v>
+      </c>
       <c r="BD18" t="s">
         <v>115</v>
       </c>
@@ -12882,6 +13267,9 @@
       <c r="BL18">
         <v>6</v>
       </c>
+      <c r="BM18" t="s">
+        <v>191</v>
+      </c>
       <c r="BO18" t="s">
         <v>133</v>
       </c>
@@ -12909,6 +13297,9 @@
       <c r="BW18">
         <v>7</v>
       </c>
+      <c r="BX18" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ18" t="s">
         <v>151</v>
       </c>
@@ -12936,6 +13327,9 @@
       <c r="CH18">
         <v>8</v>
       </c>
+      <c r="CI18" t="s">
+        <v>191</v>
+      </c>
       <c r="CK18" t="s">
         <v>169</v>
       </c>
@@ -12963,6 +13357,9 @@
       <c r="CS18">
         <v>9</v>
       </c>
+      <c r="CT18" t="s">
+        <v>190</v>
+      </c>
       <c r="CV18" t="s">
         <v>187</v>
       </c>
@@ -12990,8 +13387,11 @@
       <c r="DD18">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:108" x14ac:dyDescent="0.55000000000000004">
+      <c r="DE18" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:109" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
@@ -13019,7 +13419,9 @@
       <c r="I19" s="1">
         <v>1</v>
       </c>
-      <c r="J19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1" t="s">
         <v>44</v>
@@ -13048,7 +13450,9 @@
       <c r="T19" s="1">
         <v>2</v>
       </c>
-      <c r="U19" s="1"/>
+      <c r="U19" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="V19" s="1"/>
       <c r="W19" s="1" t="s">
         <v>62</v>
@@ -13077,7 +13481,9 @@
       <c r="AE19" s="1">
         <v>3</v>
       </c>
-      <c r="AF19" s="1"/>
+      <c r="AF19" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1" t="s">
         <v>80</v>
@@ -13106,7 +13512,9 @@
       <c r="AP19" s="1">
         <v>4</v>
       </c>
-      <c r="AQ19" s="1"/>
+      <c r="AQ19" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="AR19" s="1"/>
       <c r="AS19" s="1" t="s">
         <v>98</v>
@@ -13135,6 +13543,9 @@
       <c r="BA19" s="1">
         <v>5</v>
       </c>
+      <c r="BB19" t="s">
+        <v>191</v>
+      </c>
       <c r="BD19" t="s">
         <v>116</v>
       </c>
@@ -13162,6 +13573,9 @@
       <c r="BL19">
         <v>6</v>
       </c>
+      <c r="BM19" t="s">
+        <v>191</v>
+      </c>
       <c r="BO19" t="s">
         <v>134</v>
       </c>
@@ -13189,6 +13603,9 @@
       <c r="BW19">
         <v>7</v>
       </c>
+      <c r="BX19" t="s">
+        <v>191</v>
+      </c>
       <c r="BZ19" t="s">
         <v>152</v>
       </c>
@@ -13216,6 +13633,9 @@
       <c r="CH19">
         <v>8</v>
       </c>
+      <c r="CI19" t="s">
+        <v>191</v>
+      </c>
       <c r="CK19" t="s">
         <v>170</v>
       </c>
@@ -13243,6 +13663,9 @@
       <c r="CS19">
         <v>9</v>
       </c>
+      <c r="CT19" t="s">
+        <v>191</v>
+      </c>
       <c r="CV19" t="s">
         <v>188</v>
       </c>
@@ -13270,10 +13693,13 @@
       <c r="DD19">
         <v>10</v>
       </c>
+      <c r="DE19" t="s">
+        <v>191</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="W2:W19 L2:L19 A2:A19 AH2:AH19 AS2:AS19 BD2:BD19 BO2:BO19 BZ2:BZ19 CK2:CK19 CV2:CV19">
-    <cfRule type="duplicateValues" dxfId="40" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -31258,16 +31684,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="O110:O127">
-    <cfRule type="duplicateValues" dxfId="35" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O128:O145">
-    <cfRule type="duplicateValues" dxfId="34" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O146:O163">
-    <cfRule type="duplicateValues" dxfId="33" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O164:O181">
-    <cfRule type="duplicateValues" dxfId="32" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31277,7 +31703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D28548-4287-4DA0-B4E6-390111327B46}">
   <dimension ref="A1:W451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A223" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A434" sqref="A434:I451"/>
     </sheetView>
   </sheetViews>
@@ -49251,16 +49677,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A20:A37">
-    <cfRule type="duplicateValues" dxfId="31" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:A55">
-    <cfRule type="duplicateValues" dxfId="30" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A73">
-    <cfRule type="duplicateValues" dxfId="29" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:A91">
-    <cfRule type="duplicateValues" dxfId="28" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O20:O37">
     <cfRule type="duplicateValues" dxfId="23" priority="24"/>

</xml_diff>